<commit_message>
fixed list of figures
</commit_message>
<xml_diff>
--- a/jeng/Capstone 2 Docs/Chapters/Grammarian Feedback.xlsx
+++ b/jeng/Capstone 2 Docs/Chapters/Grammarian Feedback.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\capstone\jeng\Capstone 2 Docs\Chapters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F95B3E-3092-4A70-ACCA-D09F738DE97E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426C8676-9AE2-4091-B99D-35ADDF6010A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -858,7 +858,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B29">
         <v>5</v>

</xml_diff>